<commit_message>
added results051525.xlsx, latest results
</commit_message>
<xml_diff>
--- a/results051525.xlsx
+++ b/results051525.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dino\UCB-USACE-LSTMs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dino\USACE\UCB-USACE-LSTMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9333189-B8E8-4015-94D6-F9C5F04F7D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2700" yWindow="-21720" windowWidth="38640" windowHeight="21840"/>
+    <workbookView xWindow="-2700" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guernerville comparison" sheetId="23" r:id="rId1"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="69">
   <si>
     <t>HMS</t>
   </si>
@@ -285,11 +286,14 @@
   <si>
     <t xml:space="preserve">Daily MTS-PILSTM </t>
   </si>
+  <si>
+    <t>Contrary to expectations, several times MTS improves on LSTM, but it's likely due to the hourly longer lookback for MTS hourly (because it also has daily), and difference in hyperparameters, which may be cause by the different target variable and the stochastic variability, particularly since training is still without ensemble. The difference is alway small for daily.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -393,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -404,19 +408,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -425,18 +424,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,11 +714,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,13 +764,13 @@
       <c r="B3">
         <v>0.73237528900000004</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>0.84992650470680497</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>0.84992650470680497</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>0.84992650470680497</v>
       </c>
       <c r="F3">
@@ -792,10 +790,10 @@
       <c r="D4" s="4">
         <v>0.77870598300000005</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>0.78883092600000004</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="16">
         <v>0.87524905936336495</v>
       </c>
     </row>
@@ -803,16 +801,16 @@
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5">
         <v>0.86910101900000003</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>0.85983749600000003</v>
       </c>
       <c r="D5" s="4">
         <v>0.83485417799999995</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>0.86059591499999999</v>
       </c>
       <c r="F5" s="1">
@@ -824,7 +822,7 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -853,7 +851,7 @@
       <c r="B8">
         <v>0.87284264483909701</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>0.72606115000000004</v>
       </c>
       <c r="D8" s="4">
@@ -862,7 +860,7 @@
       <c r="E8" s="4">
         <v>0.85600518999999997</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="16">
         <v>0.89864764278509102</v>
       </c>
     </row>
@@ -873,13 +871,13 @@
       <c r="B9" s="1">
         <v>0.93125542133334305</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>0.88006156999999996</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>0.85978107299999995</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>0.88381346100000002</v>
       </c>
       <c r="F9">
@@ -1057,6 +1055,11 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1098,7 +1101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1107,213 +1110,212 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23" style="11" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="14.44140625" style="11"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10"/>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="14">
         <v>0.67838644000000003</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="14">
         <v>0.72076487</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="15">
         <v>0.75946435999999995</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="14">
         <v>115292.92200000001</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="14">
         <v>100100.986</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="15">
         <v>86227.885500000004</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="14">
         <v>339.548115</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="14">
         <v>316.38739900000002</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="15">
         <v>293.64585099999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="15">
         <v>0.76179777999999998</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
         <v>0.7460386</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="14">
         <v>0.75257715000000003</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="15">
         <v>1.1982627699999999</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <v>0.79451117000000004</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="14">
         <v>0.78865764000000005</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="14">
         <v>1.0603664500000001</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="15">
         <v>1.0049887</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="14">
         <v>0.9656827</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="14">
         <v>2.9987179999999999E-2</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="15">
         <v>2.4781500000000001E-3</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>-1.7047199999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="15">
         <v>0.88257743</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="14">
         <v>0.85084959000000004</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="14">
         <v>0.87600484999999995</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="14">
         <v>22.9739006</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="15">
         <v>-14.117378</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="15">
         <v>-14.530811</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="15">
         <v>0.43647985</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="14">
         <v>-20.260950000000001</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="14">
         <v>-19.996413</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="15">
         <v>1.6515412</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="14">
         <v>-3.4604678</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="14">
         <v>88.795782700000004</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="15">
         <v>37.443726300000002</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="14">
         <v>39.718378399999999</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="14">
         <v>42.599414699999997</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15">
         <v>-6.0366448410000002</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="1">
         <v>-0.49887032199999998</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="10">
         <v>3.431729807</v>
       </c>
     </row>
@@ -2309,7 +2311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2318,213 +2320,212 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="22" style="11" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="14.44140625" style="11"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="12">
         <v>0.737943986</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="12">
         <v>0.829204728</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <v>0.871724316</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>140274.63440000001</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>91424.134529999996</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>68664.039950000006</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>374.5325545</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>302.36424149999999</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <v>262.0382414</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>0.79139785900000004</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>0.90903868399999999</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>0.91471570000000002</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>1.180707956</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>0.99630226700000002</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>1.059315142</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>1.0379719510000001</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>0.96954242800000001</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>1.017036635</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>1.5440812999999999E-2</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>-1.2385185999999999E-2</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>6.9277319999999998E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>0.90295558300000001</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>0.91436925800000002</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <v>0.94113677799999995</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>24.529693219999999</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <v>4.8913670539999998</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>9.7088137620000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <v>23.967459529999999</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>28.48087658</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>21.948962680000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <v>78.443480440000002</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>-2303.8913910000001</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>-7.4999575580000002</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <v>0.83333333300000001</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>0.5</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>0.66666666699999999</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>45.393812570000001</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>55.886248420000001</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>45.737581579999997</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3518,7 +3519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3527,213 +3528,212 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="11" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="14.44140625" style="11"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="12">
         <v>0.61371714899999996</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="13">
         <v>0.80841976000000004</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="12">
         <v>0.798014275</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>259541.0925</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="13">
         <v>128721.59510000001</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="12">
         <v>135712.97700000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>509.45175669999998</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="13">
         <v>358.77791889999997</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>368.39242259999997</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>0.76051872099999995</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>0.88677262499999998</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>0.88789714600000003</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>1.1837439219999999</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>0.95852201599999998</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>0.96892977999999996</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>1.0379719439999999</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>1.0361848570000001</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>1.0292086300000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>1.3782000000000001E-2</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>1.3133372000000001E-2</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>1.0601335999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>0.85117935</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <v>0.90105217800000004</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>0.89632480000000003</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>25.384240630000001</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>2.1079493560000002</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>1.8262188930000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <v>31.5651154</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>-17.305943760000002</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>8.5719180680000004</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <v>79.881089040000006</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>-70.347782190000004</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>10.385102939999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>55.16080195</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>46.472183739999998</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>43.399254259999999</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="10">
         <v>-3.7971944459999998</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="10">
         <v>-3.6184856679999999</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="11">
         <v>-2.920863013</v>
       </c>
     </row>
@@ -4729,7 +4729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4921,7 +4921,7 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14">
         <v>14.6516394030394</v>
       </c>
       <c r="C14">
@@ -4952,7 +4952,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4982,7 +4982,7 @@
       <c r="C2">
         <v>0.76305628599999997</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -5173,7 +5173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5203,7 +5203,7 @@
       <c r="C2">
         <v>0.77870598300000005</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -5394,7 +5394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5424,7 +5424,7 @@
       <c r="C2">
         <v>0.78883092600000004</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -5615,7 +5615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5829,7 +5829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5859,7 +5859,7 @@
       <c r="C2" s="2">
         <v>0.72606115000000004</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -6041,7 +6041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6071,7 +6071,7 @@
       <c r="C2">
         <v>0.74605564800000002</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -6253,11 +6253,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6312,7 +6312,7 @@
       <c r="E3" s="4">
         <v>0.79554781299729505</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="12">
         <v>0.79449690699999997</v>
       </c>
     </row>
@@ -6320,19 +6320,19 @@
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4">
         <v>0.81708024721138695</v>
       </c>
       <c r="C4" s="4">
         <v>0.78109729354024504</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>0.79815864710067297</v>
       </c>
       <c r="E4" s="4">
         <v>0.78832541599999995</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="12">
         <v>0.800763691</v>
       </c>
     </row>
@@ -6340,19 +6340,19 @@
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="16">
         <v>0.80499202746418697</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>0.81021977647735299</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>0.80067638593500401</v>
       </c>
       <c r="E5" s="4">
         <v>0.78153614400000004</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="13">
         <v>0.85395714099999998</v>
       </c>
     </row>
@@ -6361,7 +6361,7 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -6379,7 +6379,7 @@
       <c r="E7" s="4">
         <v>0.75182992376732705</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="12">
         <v>0.75182992400000004</v>
       </c>
     </row>
@@ -6399,7 +6399,7 @@
       <c r="E8" s="4">
         <v>0.75451222900000003</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="12">
         <v>0.83055582299999997</v>
       </c>
     </row>
@@ -6410,16 +6410,16 @@
       <c r="B9" s="1">
         <v>0.88916793381541404</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>0.86308233599999995</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>0.89482664099999998</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>0.87491038499999996</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="17">
         <v>0.83408944500000004</v>
       </c>
     </row>
@@ -6480,7 +6480,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -6495,8 +6495,8 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>38</v>
+      <c r="A19" t="s">
+        <v>68</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -6512,7 +6512,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -6528,7 +6528,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -6544,7 +6544,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -6559,7 +6559,9 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -6593,7 +6595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6623,7 +6625,7 @@
       <c r="C2">
         <v>0.85600518999999997</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -6805,7 +6807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7018,7 +7020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7240,7 +7242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7462,7 +7464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7684,7 +7686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7897,7 +7899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8110,7 +8112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8323,7 +8325,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8536,7 +8538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8734,7 +8736,7 @@
       <c r="C14">
         <v>36.760008792817402</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14">
         <v>19.334943627581101</v>
       </c>
     </row>
@@ -8758,11 +8760,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8806,7 +8808,7 @@
       <c r="C3" s="4">
         <v>0.699238209</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="12">
         <v>0.70342375999999995</v>
       </c>
       <c r="E3" s="4"/>
@@ -8818,10 +8820,10 @@
       <c r="B4">
         <v>0.818674111593089</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>0.74070147799999997</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>0.80497083000000003</v>
       </c>
       <c r="E4" s="4"/>
@@ -8830,23 +8832,23 @@
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="16">
         <v>0.83989259939706995</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>0.829021958</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>0.84531301000000003</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -8858,7 +8860,7 @@
       <c r="C7" s="4">
         <v>0.67838644322201302</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="14">
         <v>0.67838644000000003</v>
       </c>
       <c r="E7" s="4"/>
@@ -8873,7 +8875,7 @@
       <c r="C8" s="4">
         <v>0.634547478</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>0.72076487</v>
       </c>
       <c r="E8" s="4"/>
@@ -8882,16 +8884,16 @@
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9">
         <v>0.73951758199999995</v>
       </c>
       <c r="C9" s="5">
         <v>0.75093179700000001</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="15">
         <v>0.75946435999999995</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -8949,24 +8951,13 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -8982,7 +8973,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -8998,7 +8989,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -9014,7 +9005,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -9029,7 +9020,9 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -9055,6 +9048,20 @@
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9063,7 +9070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -9324,7 +9331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9390,7 +9397,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5">
         <v>0.76179778300000001</v>
       </c>
       <c r="C5">
@@ -9404,7 +9411,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6">
         <v>1.1982627729999999</v>
       </c>
       <c r="C6">
@@ -9463,7 +9470,7 @@
       <c r="B10">
         <v>22.973900560000001</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10">
         <v>-27.792964949999998</v>
       </c>
       <c r="D10" s="1">
@@ -9488,7 +9495,7 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12">
         <v>1.6515411959999999</v>
       </c>
       <c r="C12" s="1">
@@ -9507,7 +9514,7 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14">
         <v>37.443726290000001</v>
       </c>
       <c r="C14">
@@ -9537,7 +9544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9751,7 +9758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9834,7 +9841,7 @@
       <c r="B6">
         <v>1.179486338</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6">
         <v>1.0334540560000001</v>
       </c>
       <c r="D6" s="1">
@@ -9890,7 +9897,7 @@
       <c r="B10">
         <v>24.45483673</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10">
         <v>7.6559706959999998</v>
       </c>
       <c r="D10" s="1">
@@ -9935,7 +9942,7 @@
       <c r="C13">
         <v>0.16666666699999999</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13">
         <v>0.66666666699999999</v>
       </c>
     </row>
@@ -9943,7 +9950,7 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14">
         <v>44.99523319</v>
       </c>
       <c r="C14">
@@ -9973,7 +9980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10073,7 +10080,7 @@
       <c r="C7">
         <v>1.0687861919999999</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7">
         <v>1.1015355179999999</v>
       </c>
     </row>
@@ -10188,11 +10195,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10231,7 +10238,7 @@
       <c r="B3" s="4">
         <v>0.73236276415494395</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>0.737943986</v>
       </c>
       <c r="D3" s="4"/>
@@ -10244,7 +10251,7 @@
       <c r="B4" s="4">
         <v>0.78832198710863099</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>0.829204728</v>
       </c>
       <c r="D4" s="4"/>
@@ -10257,18 +10264,18 @@
       <c r="B5" s="5">
         <v>0.85670233288490905</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="13">
         <v>0.871724316</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -10277,7 +10284,7 @@
       <c r="B7">
         <v>0.61371065199999997</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>0.61371714899999996</v>
       </c>
       <c r="D7" s="4"/>
@@ -10290,7 +10297,7 @@
       <c r="B8">
         <v>0.69504511599999996</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>0.80841976000000004</v>
       </c>
       <c r="D8" s="4"/>
@@ -10300,14 +10307,14 @@
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="18">
         <v>0.75986543600000001</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="17">
         <v>0.798014275</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -10397,7 +10404,9 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -10473,7 +10482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10482,28 +10491,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="11" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="14.44140625" style="11"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B2">
@@ -10517,7 +10525,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B3">
@@ -10531,7 +10539,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -10545,7 +10553,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
@@ -10559,7 +10567,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1">
@@ -10573,7 +10581,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
@@ -10587,7 +10595,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1">
@@ -10601,7 +10609,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B9">
@@ -10615,7 +10623,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B10">
@@ -10629,7 +10637,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B11">
@@ -10643,7 +10651,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B12">
@@ -10657,7 +10665,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B13">
@@ -10671,7 +10679,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B14">
@@ -10685,16 +10693,16 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="1">
         <v>-13.877838430000001</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15">
         <v>-16.21087966</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="10">
         <v>-17.65912462</v>
       </c>
     </row>
@@ -11690,7 +11698,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11699,28 +11707,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="22" style="11" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="14.44140625" style="11"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B2">
@@ -11734,7 +11741,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B3">
@@ -11748,7 +11755,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -11762,7 +11769,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B5">
@@ -11776,7 +11783,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B6">
@@ -11790,7 +11797,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B7">
@@ -11804,7 +11811,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
@@ -11818,7 +11825,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B9">
@@ -11832,7 +11839,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B10">
@@ -11846,7 +11853,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B11">
@@ -11860,7 +11867,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B12">
@@ -11874,15 +11881,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B14">
@@ -11896,16 +11900,16 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15">
         <v>-13.468084380000001</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="11">
         <v>-7.6200099970000004</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15">
         <v>-14.661626269999999</v>
       </c>
     </row>
@@ -12901,7 +12905,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12910,219 +12914,218 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="13" style="11" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="11" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="14.44140625" style="11"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="12">
         <v>0.79449690699999997</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="12">
         <v>0.800763691</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <v>0.85395714099999998</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>408094.8456</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>395650.0577</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>290016.7438</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>638.82301589999997</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>629.00720009999998</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <v>538.53202669999996</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>0.72784005799999996</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>0.79796283599999995</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>0.83546030900000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>1.1869242900000001</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>0.95804508200000005</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>0.949108014</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>1.185326973</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>1.1703163080000001</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>1.1380212220000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>7.9795238000000004E-2</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>7.3332176999999998E-2</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>5.9427054999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="13">
         <v>0.930831678</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>0.89974454800000003</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>0.92628800499999997</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>23.955099950000001</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <v>-1.670300793</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>-2.9504457020000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="13">
         <v>31.74487225</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>33.789893229999997</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>33.651381720000003</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="13">
         <v>96.362760100000003</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>99.108365800000001</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>98.156697480000005</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <v>0.2</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>0</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>37.534168090000001</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>49.125625769999999</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>35.40779208</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15">
         <v>-18.532697280000001</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="10">
         <v>-17.031630799999999</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="1">
         <v>-13.80212216</v>
       </c>
     </row>
@@ -14118,7 +14121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14127,213 +14130,212 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" style="11" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="14.44140625" style="11"/>
+    <col min="1" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="12">
         <v>0.75182992400000004</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="12">
         <v>0.83055582299999997</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <v>0.83408944500000004</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>549210.37840000005</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>374986.7917</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>367166.74430000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>741.0872948</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>612.36165110000002</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <v>605.9428557</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>0.71182068300000001</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>0.83187909699999996</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>0.83484145200000004</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>1.204127553</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>0.88414415899999999</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>0.928647365</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>1.1855502950000001</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <v>1.0847093670000001</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>1.122140666</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>7.5688790000000006E-2</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>3.455424E-2</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>4.9823037000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="13">
         <v>0.91663124699999998</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>0.91244210299999995</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>0.91474857499999995</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>22.67961352</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>-9.8381072389999993</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>-5.2893476619999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <v>26.515350470000001</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <v>6.5505512460000004</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>30.283703500000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <v>96.357821479999998</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>-1.791996465</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>-1.334565673</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>40.299279390000002</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>32.916508</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>28.573038919999998</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15">
         <v>-18.555029480000002</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="11">
         <v>-8.4709367419999992</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15">
         <v>-12.21406657</v>
       </c>
     </row>
@@ -15329,7 +15331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15338,219 +15340,218 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="11" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="14.44140625" style="11"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="12">
         <v>0.70342375999999995</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="12">
         <v>0.80497083000000003</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <v>0.84531301000000003</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>75747.091499999995</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>49811.448600000003</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>39507.849000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>275.22189500000002</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>223.184786</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <v>198.76581400000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>0.74807279000000004</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>0.78070702000000003</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>0.86445622</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>1.22328338</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>0.80349486999999997</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>0.89084280000000005</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>1.0595205400000001</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <v>0.99887146999999998</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>1.0060556199999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>3.4922109999999999E-2</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>-6.6209999999999999E-4</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>3.5529799999999999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>0.89965481000000003</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>0.90266617000000005</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <v>0.91987414999999995</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>25.178583199999998</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>-17.956762000000001</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>-5.2211290000000004</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="13">
         <v>0.13513965</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>-20.152343999999999</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>-28.321929999999998</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <v>-969.89094</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <v>-11.874632999999999</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>59.361660999999998</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <v>0</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>0.4</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>54.494070800000003</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>39.046320600000001</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>19.7078186</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="10">
         <v>-5.952053727</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="1">
         <v>0.112853245</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15">
         <v>-0.60556242299999996</v>
       </c>
     </row>

</xml_diff>